<commit_message>
Code Contest Tool v0.2
</commit_message>
<xml_diff>
--- a/code-contest/code-contest.xlsx
+++ b/code-contest/code-contest.xlsx
@@ -2,24 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kljh\Documents\Code\GitHub\webapp\code-contest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:400001_{6B7F1813-E93B-4C34-8CED-71B7E36B406E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:400001_{603B3CDF-A9FF-44A7-8938-180596EAFB16}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5268" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5268" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
     <sheet name="Setup" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
     <definedName name="db">Setup!$C$2</definedName>
+    <definedName name="http_pwd">Setup!$C$5</definedName>
+    <definedName name="http_query">Setup!$R$2</definedName>
+    <definedName name="http_server">Setup!$C$3</definedName>
+    <definedName name="http_user">Setup!$C$4</definedName>
   </definedNames>
   <calcPr calcId="171027" refMode="R1C1"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t xml:space="preserve">generate attempt submission number </t>
   </si>
@@ -204,9 +212,6 @@
     <t>submissions</t>
   </si>
   <si>
-    <t>db</t>
-  </si>
-  <si>
     <t>C:\Users\kljh\Documents\Code\GitHub\webapp\code-contest\.code-contest\db.sqlite</t>
   </si>
   <si>
@@ -280,13 +285,52 @@
   </si>
   <si>
     <t>o2</t>
+  </si>
+  <si>
+    <t>local db</t>
+  </si>
+  <si>
+    <t>kljh</t>
+  </si>
+  <si>
+    <t>http server</t>
+  </si>
+  <si>
+    <t>http query</t>
+  </si>
+  <si>
+    <t>http://localhost:8085/</t>
+  </si>
+  <si>
+    <t>sqlite_exec?db=code-contest/.code-contest/db.sqlite&amp;to_tsv=true&amp;stmt=</t>
+  </si>
+  <si>
+    <t>http stmt</t>
+  </si>
+  <si>
+    <t>http user</t>
+  </si>
+  <si>
+    <t>http pwd</t>
+  </si>
+  <si>
+    <t>select * from problems</t>
+  </si>
+  <si>
+    <t>=XlSQLiteTable(db,RC[-1],XlAutoCrop(R[1]C[-2]:R[23]C))</t>
+  </si>
+  <si>
+    <t>regstress</t>
+  </si>
+  <si>
+    <t>---</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +342,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -409,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -427,6 +479,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1601,6 +1655,22 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="HttpRequest"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1900,9 +1970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="C3:U30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2006,10 +2077,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E43363-9F66-4EA1-81A4-2C14309DA540}">
-  <dimension ref="B2:O27"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="B2:U30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2023,314 +2095,371 @@
     <col min="13" max="13" width="12.109375" customWidth="1"/>
     <col min="14" max="14" width="15.77734375" customWidth="1"/>
     <col min="15" max="15" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="R3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" t="str">
+        <f>[1]!HttpRequest(http_server&amp;"sqlite_table?db=code-contest/.code-contest/db.sqlite&amp;table="&amp;N7,M8:O12,http_user,http_pwd)</f>
+        <v>401 Unauthorized</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="b">
+        <f ca="1">_xll.XlSQLiteTable(db,C7,_xll.XlAutoCrop(B8:G30))</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="b">
-        <f ca="1">_xll.XlSQLiteTable(db,C4,_xll.XlAutoCrop(B5:G27))</f>
+      <c r="K7" t="b">
+        <f>_xll.XlSQLiteTable(db,J7,_xll.XlAutoCrop(I8:K30))</f>
         <v>1</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="M7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K4" t="b">
-        <f>_xll.XlSQLiteTable(db,J4,_xll.XlAutoCrop(I5:K27))</f>
-        <v>1</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="M8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q8" s="12" t="str">
+        <f t="array" ref="Q8:U30">[1]!HttpRequest(http_server&amp;http_query&amp;R3,,http_user,http_pwd)</f>
+        <v>401 Unauthorized</v>
+      </c>
+      <c r="R8" s="13" t="str">
+        <v>401 Unauthorized</v>
+      </c>
+      <c r="S8" s="13" t="str">
+        <v>401 Unauthorized</v>
+      </c>
+      <c r="T8" s="13" t="str">
+        <v>401 Unauthorized</v>
+      </c>
+      <c r="U8" s="14" t="str">
+        <v>401 Unauthorized</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="O4" t="b">
-        <f>_xll.XlSQLiteTable(db,N4,_xll.XlAutoCrop(M5:O27))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="11">
-        <v>43229.059239004629</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5">
-        <v>3.14</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="11">
-        <f t="shared" ref="E7:E8" ca="1" si="0">E6+RAND()/300</f>
-        <v>43229.061168945846</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G7" s="5">
-        <v>4.7</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="11">
-        <f t="shared" ref="E8" ca="1" si="1">E7+RAND()/300</f>
-        <v>43229.061865271091</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="5">
-        <v>3.6</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="O8" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>46</v>
       </c>
       <c r="E9" s="11">
-        <f t="shared" ref="E9" ca="1" si="2">E8+RAND()/300</f>
-        <v>43229.064324437873</v>
+        <v>43229.059239004629</v>
       </c>
       <c r="F9" s="3">
         <v>1</v>
       </c>
       <c r="G9" s="5">
+        <v>3.14</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
+        <v>0</v>
+      </c>
+      <c r="S9" s="3">
+        <v>0</v>
+      </c>
+      <c r="T9" s="3">
+        <v>0</v>
+      </c>
+      <c r="U9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" ref="E10" ca="1" si="0">E9+RAND()/300</f>
+        <v>43229.060094931971</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="5">
+        <v>4.7</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="O10" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R10" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S10" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T10" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U10" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="11">
+        <f t="shared" ref="E11" ca="1" si="1">E10+RAND()/300</f>
+        <v>43229.063317831453</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="5">
+        <v>3.6</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="O11" s="5">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R11" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S11" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T11" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U11" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="11">
+        <f t="shared" ref="E12" ca="1" si="2">E11+RAND()/300</f>
+        <v>43229.065349376251</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
         <v>3.15</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="5"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="11">
-        <f ca="1">E7+RAND()/300</f>
-        <v>43229.064143892254</v>
-      </c>
-      <c r="F10" s="10">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="5"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="11">
-        <f ca="1">E8+RAND()/300</f>
-        <v>43229.063840753937</v>
-      </c>
-      <c r="F11" s="10">
-        <v>1</v>
-      </c>
-      <c r="G11" s="5">
-        <v>3.14159276</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="5"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="11">
-        <f ca="1">E9+RAND()/300</f>
-        <v>43229.065256380432</v>
-      </c>
-      <c r="F12" s="10">
-        <v>1</v>
-      </c>
-      <c r="G12" s="5">
-        <v>3.1419999999999999</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="3"/>
       <c r="K12" s="5"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="5"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="6"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="M12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="O12" s="5">
+        <v>7</v>
+      </c>
+      <c r="Q12" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R12" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S12" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T12" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U12" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="11">
+        <f ca="1">E10+RAND()/300</f>
+        <v>43229.063151196402</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
       <c r="G13" s="5"/>
       <c r="I13" s="6"/>
       <c r="J13" s="3"/>
@@ -2338,36 +2467,107 @@
       <c r="M13" s="6"/>
       <c r="N13" s="3"/>
       <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="6"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="5"/>
+      <c r="Q13" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R13" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S13" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T13" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U13" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="11">
+        <f ca="1">E11+RAND()/300</f>
+        <v>43229.064622380618</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>3.14159276</v>
+      </c>
       <c r="I14" s="6"/>
       <c r="J14" s="3"/>
       <c r="K14" s="5"/>
       <c r="M14" s="6"/>
       <c r="N14" s="3"/>
       <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="6"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="5"/>
+      <c r="Q14" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R14" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S14" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T14" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U14" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="11">
+        <f ca="1">E12+RAND()/300</f>
+        <v>43229.066697124821</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <v>3.1419999999999999</v>
+      </c>
       <c r="I15" s="6"/>
       <c r="J15" s="3"/>
       <c r="K15" s="5"/>
       <c r="M15" s="6"/>
       <c r="N15" s="3"/>
       <c r="O15" s="5"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q15" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R15" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S15" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T15" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U15" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -2380,8 +2580,23 @@
       <c r="M16" s="6"/>
       <c r="N16" s="3"/>
       <c r="O16" s="5"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q16" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R16" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S16" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T16" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U16" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B17" s="6"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2394,8 +2609,23 @@
       <c r="M17" s="6"/>
       <c r="N17" s="3"/>
       <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q17" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R17" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S17" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T17" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U17" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2408,8 +2638,23 @@
       <c r="M18" s="6"/>
       <c r="N18" s="3"/>
       <c r="O18" s="5"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q18" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R18" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S18" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T18" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U18" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B19" s="6"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -2422,8 +2667,23 @@
       <c r="M19" s="6"/>
       <c r="N19" s="3"/>
       <c r="O19" s="5"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q19" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R19" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S19" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T19" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U19" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2436,8 +2696,23 @@
       <c r="M20" s="6"/>
       <c r="N20" s="3"/>
       <c r="O20" s="5"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q20" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R20" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S20" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T20" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U20" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B21" s="6"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2450,8 +2725,23 @@
       <c r="M21" s="6"/>
       <c r="N21" s="3"/>
       <c r="O21" s="5"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q21" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R21" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S21" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T21" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U21" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B22" s="6"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2464,8 +2754,23 @@
       <c r="M22" s="6"/>
       <c r="N22" s="3"/>
       <c r="O22" s="5"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q22" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R22" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S22" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T22" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U22" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -2478,8 +2783,23 @@
       <c r="M23" s="6"/>
       <c r="N23" s="3"/>
       <c r="O23" s="5"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q23" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R23" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S23" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T23" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U23" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B24" s="6"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -2492,8 +2812,23 @@
       <c r="M24" s="6"/>
       <c r="N24" s="3"/>
       <c r="O24" s="5"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q24" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R24" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S24" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T24" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U24" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B25" s="6"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -2506,8 +2841,23 @@
       <c r="M25" s="6"/>
       <c r="N25" s="3"/>
       <c r="O25" s="5"/>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="Q25" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R25" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S25" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T25" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U25" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B26" s="6"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2520,22 +2870,144 @@
       <c r="M26" s="6"/>
       <c r="N26" s="3"/>
       <c r="O26" s="5"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="9"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="9"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="9"/>
+      <c r="Q26" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R26" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S26" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T26" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U26" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B27" s="6"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="5"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="5"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="5"/>
+      <c r="Q27" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R27" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S27" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T27" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U27" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B28" s="6"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="5"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="5"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="5"/>
+      <c r="Q28" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R28" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S28" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T28" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U28" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B29" s="6"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="5"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="5"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="5"/>
+      <c r="Q29" s="6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R29" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S29" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T29" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U29" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="9"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="9"/>
+      <c r="Q30" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R30" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S30" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T30" s="8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U30" s="9" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C3" xr:uid="{338B2B33-39E0-4B25-A745-FD05625E4B4F}">
+      <formula1>"http://kljh.herokuapp.com/,http://localhost:8085/"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Code Contest - sched problem scoring
</commit_message>
<xml_diff>
--- a/code-contest/code-contest.xlsx
+++ b/code-contest/code-contest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kljh\Documents\Code\GitHub\webapp\code-contest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722F7822-3804-4F5D-93C4-A427591846E0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:400001_{5BAB2479-57DF-4F16-9CBB-E3E689B5053B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5268" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5268" tabRatio="624" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="93">
   <si>
     <t xml:space="preserve">generate attempt submission number </t>
   </si>
@@ -381,6 +381,45 @@
   <si>
     <t>struct</t>
   </si>
+  <si>
+    <t>Algo exec time</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>| user_id | Max(NbSolved) |</t>
+  </si>
+  <si>
+    <t>| me | 8 |</t>
+  </si>
+  <si>
+    <t>| Los_Macholos_de_la_Programacion | 8 |</t>
+  </si>
+  <si>
+    <t>| ajesus | 9 |</t>
+  </si>
+  <si>
+    <t>| pedro | 13 |</t>
+  </si>
+  <si>
+    <t>| kljh | 14 |</t>
+  </si>
+  <si>
+    <t>| shotless | 22 |</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
 </sst>
 </file>
 
@@ -523,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,6 +616,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="45" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2073,9 +2124,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="C3:U30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2182,8 +2231,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:X84"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView showGridLines="0" topLeftCell="N52" workbookViewId="0">
+      <selection activeCell="X84" sqref="X84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5331,9 +5380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE2FAB5-253A-4FE2-B785-D89344B47279}">
   <dimension ref="B2:K79"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7881,55 +7928,55 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9DBE86-C2FF-493E-B264-86696866C972}">
-  <dimension ref="A2:O163"/>
+  <dimension ref="A2:M163"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="34.44140625" customWidth="1"/>
     <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
     <col min="6" max="10" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.77734375" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="str">
-        <f t="array" aca="1" ref="B3" ca="1">"select user_id, problem_id, substr(timestamp,12,8) as time, completed, count(result), sum(result), min(result), max(result), avg(result) from submissions  where attempt &gt; 'ATTEMPT-2018-12-13'  and problem_id = '"&amp;A6&amp;"' group by attempt order by attempt desc"</f>
-        <v>select user_id, problem_id, substr(timestamp,12,8) as time, completed, count(result), sum(result), min(result), max(result), avg(result) from submissions  where attempt &gt; 'ATTEMPT-2018-12-13'  and problem_id = 'yap' group by attempt order by attempt desc</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <f ca="1">"select user_id, problem_id, substr(min(timestamp),12,8) as t0,  substr(max(timestamp),12,8) as t1, count(result), sum(result), min(result), max(result), avg(result) from submissions  where attempt &gt; 'ATTEMPT-2018-12-13'  and problem_id = '"&amp;A7&amp;"' group by attempt order by attempt desc"</f>
+        <v>select user_id, problem_id, substr(min(timestamp),12,8) as t0,  substr(max(timestamp),12,8) as t1, count(result), sum(result), min(result), max(result), avg(result) from submissions  where attempt &gt; 'ATTEMPT-2018-12-13'  and problem_id = 'sched' group by attempt order by attempt desc</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>79</v>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>77</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="str">
         <f t="array" aca="1" ref="B9:J163" ca="1">_xll.XlAutoFit(_xll.XlSQLiteExec(db,Porto!$B$3))</f>
         <v>user_id</v>
@@ -7940,11 +7987,11 @@
       </c>
       <c r="D9" s="13" t="str">
         <f ca="1"/>
-        <v>time</v>
+        <v>t0</v>
       </c>
       <c r="E9" s="13" t="str">
         <f ca="1"/>
-        <v>completed</v>
+        <v>t1</v>
       </c>
       <c r="F9" s="29" t="str">
         <f ca="1"/>
@@ -7966,1717 +8013,1639 @@
         <f ca="1"/>
         <v>avg(result)</v>
       </c>
-      <c r="L9" t="str">
-        <f t="array" aca="1" ref="L9:M19" ca="1">_xll.XlSQLite(B9:E163, "select distinct user_id from data")</f>
-        <v>user_id</v>
-      </c>
-      <c r="M9" t="str">
-        <f ca="1"/>
-        <v>user_id</v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" ref="O9:O10" ca="1" si="0">"| "&amp;B9&amp;" | "&amp;C9&amp;" |"</f>
-        <v>| user_id | Max(NbSolved) |</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L9" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="M9" s="30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="str">
         <f ca="1"/>
-        <v>casa519</v>
+        <v>test-emm</v>
       </c>
       <c r="C10" s="24" t="str">
         <f ca="1"/>
-        <v>yap</v>
+        <v>sched</v>
       </c>
       <c r="D10" s="24" t="str">
         <f ca="1"/>
-        <v>18:33:13</v>
-      </c>
-      <c r="E10" s="24">
-        <f ca="1"/>
-        <v>0.5</v>
+        <v>22:37:29</v>
+      </c>
+      <c r="E10" s="24" t="str">
+        <f ca="1"/>
+        <v>22:38:10</v>
       </c>
       <c r="F10" s="31">
         <f ca="1"/>
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="G10" s="31">
         <f ca="1"/>
-        <v>207</v>
+        <v>2672192</v>
       </c>
       <c r="H10" s="31">
         <f ca="1"/>
-        <v>21</v>
+        <v>85664</v>
       </c>
       <c r="I10" s="31">
         <f ca="1"/>
-        <v>84</v>
+        <v>86360</v>
       </c>
       <c r="J10" s="32">
         <f ca="1"/>
-        <v>41.4</v>
-      </c>
-      <c r="L10" t="str">
+        <v>86199.741935483864</v>
+      </c>
+      <c r="L10" s="39">
+        <f t="shared" ref="L10:L13" ca="1" si="0">E10-D10</f>
+        <v>4.7453703703714822E-4</v>
+      </c>
+      <c r="M10" s="32">
+        <f t="shared" ref="M10:M13" ca="1" si="1">86400*F10-G10</f>
+        <v>6208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="23" t="str">
+        <f ca="1"/>
+        <v>test-draginoi</v>
+      </c>
+      <c r="C11" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D11" s="24" t="str">
+        <f ca="1"/>
+        <v>22:33:12</v>
+      </c>
+      <c r="E11" s="24" t="str">
+        <f ca="1"/>
+        <v>22:33:56</v>
+      </c>
+      <c r="F11" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G11" s="31">
+        <f ca="1"/>
+        <v>86330</v>
+      </c>
+      <c r="H11" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I11" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J11" s="32">
+        <f ca="1"/>
+        <v>2784.8387096774195</v>
+      </c>
+      <c r="L11" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.0925925925926485E-4</v>
+      </c>
+      <c r="M11" s="32">
+        <f t="shared" ca="1" si="1"/>
+        <v>2592070</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="23" t="str">
+        <f ca="1"/>
+        <v>test-Global_Domination</v>
+      </c>
+      <c r="C12" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D12" s="24" t="str">
+        <f ca="1"/>
+        <v>22:32:30</v>
+      </c>
+      <c r="E12" s="24" t="str">
+        <f ca="1"/>
+        <v>22:33:09</v>
+      </c>
+      <c r="F12" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G12" s="31">
+        <f ca="1"/>
+        <v>2673419</v>
+      </c>
+      <c r="H12" s="31">
+        <f ca="1"/>
+        <v>85664</v>
+      </c>
+      <c r="I12" s="31">
+        <f ca="1"/>
+        <v>86364</v>
+      </c>
+      <c r="J12" s="32">
+        <f ca="1"/>
+        <v>86239.322580645166</v>
+      </c>
+      <c r="L12" s="39">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.5138888888873741E-4</v>
+      </c>
+      <c r="M12" s="32">
+        <f t="shared" ca="1" si="1"/>
+        <v>4981</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="23" t="str">
+        <f ca="1"/>
+        <v>test-Dino-Team</v>
+      </c>
+      <c r="C13" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D13" s="24" t="str">
+        <f ca="1"/>
+        <v>22:31:24</v>
+      </c>
+      <c r="E13" s="24" t="str">
+        <f ca="1"/>
+        <v>22:32:25</v>
+      </c>
+      <c r="F13" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G13" s="31">
+        <f ca="1"/>
+        <v>2668319</v>
+      </c>
+      <c r="H13" s="31">
+        <f ca="1"/>
+        <v>85664</v>
+      </c>
+      <c r="I13" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J13" s="32">
+        <f ca="1"/>
+        <v>86074.806451612909</v>
+      </c>
+      <c r="L13" s="40">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.0601851851848085E-4</v>
+      </c>
+      <c r="M13" s="38">
+        <f t="shared" ca="1" si="1"/>
+        <v>10081</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="23" t="str">
         <f ca="1"/>
         <v>Dino-Team</v>
       </c>
-      <c r="M10" t="str">
+      <c r="C14" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D14" s="24" t="str">
+        <f ca="1"/>
+        <v>19:04:03</v>
+      </c>
+      <c r="E14" s="24" t="str">
+        <f ca="1"/>
+        <v>19:04:10</v>
+      </c>
+      <c r="F14" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G14" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H14" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I14" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J14" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="23" t="str">
         <f ca="1"/>
         <v>Dino-Team</v>
       </c>
-      <c r="O10" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>| shotless | 22 |</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="str">
-        <f ca="1"/>
-        <v>casa519</v>
-      </c>
-      <c r="C11" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D11" s="24" t="str">
-        <f ca="1"/>
-        <v>18:30:44</v>
-      </c>
-      <c r="E11" s="24">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="31">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G11" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="H11" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="I11" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="J11" s="32">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="L11" t="str">
+      <c r="C15" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D15" s="24" t="str">
+        <f ca="1"/>
+        <v>19:02:33</v>
+      </c>
+      <c r="E15" s="24" t="str">
+        <f ca="1"/>
+        <v>19:02:41</v>
+      </c>
+      <c r="F15" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G15" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H15" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I15" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J15" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="23" t="str">
+        <f ca="1"/>
+        <v>Dino-Team</v>
+      </c>
+      <c r="C16" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D16" s="24" t="str">
+        <f ca="1"/>
+        <v>18:56:15</v>
+      </c>
+      <c r="E16" s="24" t="str">
+        <f ca="1"/>
+        <v>18:56:23</v>
+      </c>
+      <c r="F16" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G16" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H16" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I16" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J16" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="23" t="str">
         <f ca="1"/>
         <v>Global_Domination</v>
       </c>
-      <c r="M11" t="str">
+      <c r="C17" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D17" s="24" t="str">
+        <f ca="1"/>
+        <v>18:49:16</v>
+      </c>
+      <c r="E17" s="24" t="str">
+        <f ca="1"/>
+        <v>18:49:25</v>
+      </c>
+      <c r="F17" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G17" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H17" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I17" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J17" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="23" t="str">
+        <f ca="1"/>
+        <v>Dino-Team</v>
+      </c>
+      <c r="C18" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D18" s="24" t="str">
+        <f ca="1"/>
+        <v>18:47:21</v>
+      </c>
+      <c r="E18" s="24" t="str">
+        <f ca="1"/>
+        <v>18:47:30</v>
+      </c>
+      <c r="F18" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G18" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H18" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I18" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J18" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="23" t="str">
+        <f ca="1"/>
+        <v>emm</v>
+      </c>
+      <c r="C19" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D19" s="24" t="str">
+        <f ca="1"/>
+        <v>18:46:41</v>
+      </c>
+      <c r="E19" s="24" t="str">
+        <f ca="1"/>
+        <v>18:46:48</v>
+      </c>
+      <c r="F19" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G19" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H19" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I19" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J19" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="23" t="str">
+        <f ca="1"/>
+        <v>Dino-Team</v>
+      </c>
+      <c r="C20" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D20" s="24" t="str">
+        <f ca="1"/>
+        <v>18:42:09</v>
+      </c>
+      <c r="E20" s="24" t="str">
+        <f ca="1"/>
+        <v>18:42:16</v>
+      </c>
+      <c r="F20" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G20" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H20" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I20" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J20" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="23" t="str">
+        <f ca="1"/>
+        <v>Dino-Team</v>
+      </c>
+      <c r="C21" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D21" s="24" t="str">
+        <f ca="1"/>
+        <v>18:41:35</v>
+      </c>
+      <c r="E21" s="24" t="str">
+        <f ca="1"/>
+        <v>18:41:42</v>
+      </c>
+      <c r="F21" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G21" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H21" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I21" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J21" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="23" t="str">
+        <f ca="1"/>
+        <v>Dino-Team</v>
+      </c>
+      <c r="C22" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D22" s="24" t="str">
+        <f ca="1"/>
+        <v>18:41:12</v>
+      </c>
+      <c r="E22" s="24" t="str">
+        <f ca="1"/>
+        <v>18:41:19</v>
+      </c>
+      <c r="F22" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G22" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H22" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I22" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J22" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="23" t="str">
         <f ca="1"/>
         <v>Global_Domination</v>
       </c>
-      <c r="O11" t="str">
-        <f ca="1">"| "&amp;B11&amp;" | "&amp;C11&amp;" |"</f>
-        <v>| kljh | 14 |</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="str">
+      <c r="C23" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D23" s="24" t="str">
+        <f ca="1"/>
+        <v>18:40:56</v>
+      </c>
+      <c r="E23" s="24" t="str">
+        <f ca="1"/>
+        <v>18:41:06</v>
+      </c>
+      <c r="F23" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G23" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H23" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I23" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J23" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="23" t="str">
         <f ca="1"/>
         <v>Dino-Team</v>
       </c>
-      <c r="C12" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D12" s="24" t="str">
-        <f ca="1"/>
-        <v>18:29:54</v>
-      </c>
-      <c r="E12" s="24">
-        <f ca="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="F12" s="31">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="G12" s="31">
-        <f ca="1"/>
-        <v>177</v>
-      </c>
-      <c r="H12" s="31">
-        <f ca="1"/>
-        <v>25</v>
-      </c>
-      <c r="I12" s="31">
-        <f ca="1"/>
-        <v>46</v>
-      </c>
-      <c r="J12" s="32">
-        <f ca="1"/>
-        <v>35.4</v>
-      </c>
-      <c r="L12" t="str">
-        <f ca="1"/>
-        <v>emm</v>
-      </c>
-      <c r="M12" t="str">
-        <f ca="1"/>
-        <v>emm</v>
-      </c>
-      <c r="O12" t="str">
-        <f ca="1">"| "&amp;B12&amp;" | "&amp;C12&amp;" |"</f>
-        <v>| pedro | 13 |</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="23" t="str">
+      <c r="C24" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D24" s="24" t="str">
+        <f ca="1"/>
+        <v>18:40:52</v>
+      </c>
+      <c r="E24" s="24" t="str">
+        <f ca="1"/>
+        <v>18:41:03</v>
+      </c>
+      <c r="F24" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G24" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H24" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I24" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J24" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="23" t="str">
         <f ca="1"/>
         <v>Global_Domination</v>
       </c>
-      <c r="C13" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D13" s="24" t="str">
-        <f ca="1"/>
-        <v>17:04:04</v>
-      </c>
-      <c r="E13" s="24">
-        <f ca="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="F13" s="31">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="G13" s="31">
-        <f ca="1"/>
-        <v>163</v>
-      </c>
-      <c r="H13" s="31">
-        <f ca="1"/>
-        <v>23</v>
-      </c>
-      <c r="I13" s="31">
-        <f ca="1"/>
-        <v>45</v>
-      </c>
-      <c r="J13" s="32">
-        <f ca="1"/>
-        <v>32.6</v>
-      </c>
-      <c r="L13" t="str">
+      <c r="C25" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D25" s="24" t="str">
+        <f ca="1"/>
+        <v>18:36:19</v>
+      </c>
+      <c r="E25" s="24" t="str">
+        <f ca="1"/>
+        <v>18:36:25</v>
+      </c>
+      <c r="F25" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G25" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H25" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I25" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J25" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="23" t="str">
+        <f ca="1"/>
+        <v>Dino-Team</v>
+      </c>
+      <c r="C26" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D26" s="24" t="str">
+        <f ca="1"/>
+        <v>18:35:59</v>
+      </c>
+      <c r="E26" s="24" t="str">
+        <f ca="1"/>
+        <v>18:36:07</v>
+      </c>
+      <c r="F26" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G26" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H26" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I26" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J26" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="23" t="str">
         <f ca="1"/>
         <v>draginoi</v>
       </c>
-      <c r="M13" t="str">
-        <f ca="1"/>
-        <v>draginoi</v>
-      </c>
-      <c r="O13" t="str">
-        <f ca="1">"| "&amp;B13&amp;" | "&amp;C13&amp;" |"</f>
-        <v>| ajesus | 9 |</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="23" t="str">
+      <c r="C27" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D27" s="24" t="str">
+        <f ca="1"/>
+        <v>18:35:23</v>
+      </c>
+      <c r="E27" s="24" t="str">
+        <f ca="1"/>
+        <v>18:35:26</v>
+      </c>
+      <c r="F27" s="31">
+        <f ca="1"/>
+        <v>19</v>
+      </c>
+      <c r="G27" s="31">
+        <f ca="1"/>
+        <v>86342</v>
+      </c>
+      <c r="H27" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I27" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J27" s="32">
+        <f ca="1"/>
+        <v>4544.3157894736842</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="23" t="str">
         <f ca="1"/>
         <v>Dino-Team</v>
       </c>
-      <c r="C14" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D14" s="24" t="str">
-        <f ca="1"/>
-        <v>16:36:14</v>
-      </c>
-      <c r="E14" s="24">
-        <f ca="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="F14" s="31">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="G14" s="31">
-        <f ca="1"/>
-        <v>143</v>
-      </c>
-      <c r="H14" s="31">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="I14" s="31">
-        <f ca="1"/>
-        <v>50</v>
-      </c>
-      <c r="J14" s="32">
-        <f ca="1"/>
-        <v>28.6</v>
-      </c>
-      <c r="L14" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="M14" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="O14" t="str">
-        <f ca="1">"| "&amp;B14&amp;" | "&amp;C14&amp;" |"</f>
-        <v>| Los_Macholos_de_la_Programacion | 8 |</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="23" t="str">
+      <c r="C28" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D28" s="24" t="str">
+        <f ca="1"/>
+        <v>18:34:37</v>
+      </c>
+      <c r="E28" s="24" t="str">
+        <f ca="1"/>
+        <v>18:34:45</v>
+      </c>
+      <c r="F28" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G28" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H28" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I28" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J28" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="23" t="str">
         <f ca="1"/>
         <v>Dino-Team</v>
       </c>
-      <c r="C15" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D15" s="24" t="str">
-        <f ca="1"/>
-        <v>16:24:01</v>
-      </c>
-      <c r="E15" s="24">
-        <f ca="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="F15" s="31">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="G15" s="31">
-        <f ca="1"/>
-        <v>243</v>
-      </c>
-      <c r="H15" s="31">
-        <f ca="1"/>
-        <v>2</v>
-      </c>
-      <c r="I15" s="31">
-        <f ca="1"/>
-        <v>90</v>
-      </c>
-      <c r="J15" s="32">
-        <f ca="1"/>
-        <v>48.6</v>
-      </c>
-      <c r="L15" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M15" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="O15" t="str">
-        <f ca="1">"| "&amp;B15&amp;" | "&amp;C15&amp;" |"</f>
-        <v>| me | 8 |</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="23" t="str">
+      <c r="C29" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D29" s="24" t="str">
+        <f ca="1"/>
+        <v>18:31:52</v>
+      </c>
+      <c r="E29" s="24" t="str">
+        <f ca="1"/>
+        <v>18:31:59</v>
+      </c>
+      <c r="F29" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G29" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H29" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I29" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J29" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="23" t="str">
         <f ca="1"/>
         <v>Dino-Team</v>
       </c>
-      <c r="C16" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D16" s="24" t="str">
-        <f ca="1"/>
-        <v>16:15:46</v>
-      </c>
-      <c r="E16" s="24">
-        <f ca="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="F16" s="31">
-        <f ca="1"/>
-        <v>5</v>
-      </c>
-      <c r="G16" s="31">
-        <f ca="1"/>
-        <v>245</v>
-      </c>
-      <c r="H16" s="31">
-        <f ca="1"/>
-        <v>6</v>
-      </c>
-      <c r="I16" s="31">
-        <f ca="1"/>
-        <v>93</v>
-      </c>
-      <c r="J16" s="32">
-        <f ca="1"/>
-        <v>49</v>
-      </c>
-      <c r="L16" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M16" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="23" t="str">
+      <c r="C30" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D30" s="24" t="str">
+        <f ca="1"/>
+        <v>18:31:37</v>
+      </c>
+      <c r="E30" s="24" t="str">
+        <f ca="1"/>
+        <v>18:31:42</v>
+      </c>
+      <c r="F30" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G30" s="31">
+        <f ca="1"/>
+        <v>-31</v>
+      </c>
+      <c r="H30" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I30" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J30" s="32">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="23" t="str">
         <f ca="1"/>
         <v>Dino-Team</v>
       </c>
-      <c r="C17" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D17" s="24" t="str">
-        <f ca="1"/>
-        <v>16:12:01</v>
-      </c>
-      <c r="E17" s="24">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="31">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G17" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="H17" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="I17" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="J17" s="32">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="L17" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M17" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="23" t="str">
-        <f ca="1"/>
-        <v>Dino-Team</v>
-      </c>
-      <c r="C18" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D18" s="24" t="str">
-        <f ca="1"/>
-        <v>16:04:01</v>
-      </c>
-      <c r="E18" s="24">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="31">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G18" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="H18" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="I18" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="J18" s="32">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="L18" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M18" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="23" t="str">
-        <f ca="1"/>
-        <v>Dino-Team</v>
-      </c>
-      <c r="C19" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D19" s="24" t="str">
-        <f ca="1"/>
-        <v>16:00:38</v>
-      </c>
-      <c r="E19" s="24">
-        <f ca="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="F19" s="31">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H19" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I19" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J19" s="32" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="L19" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M19" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="23" t="str">
-        <f ca="1"/>
-        <v>Dino-Team</v>
-      </c>
-      <c r="C20" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D20" s="24" t="str">
-        <f ca="1"/>
-        <v>15:58:07</v>
-      </c>
-      <c r="E20" s="24">
-        <f ca="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="F20" s="31">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H20" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I20" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J20" s="32" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="23" t="str">
-        <f ca="1"/>
-        <v>Dino-Team</v>
-      </c>
-      <c r="C21" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D21" s="24" t="str">
-        <f ca="1"/>
-        <v>15:57:26</v>
-      </c>
-      <c r="E21" s="24">
-        <f ca="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="F21" s="31">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H21" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I21" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J21" s="32" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="23" t="str">
+      <c r="C31" s="24" t="str">
+        <f ca="1"/>
+        <v>sched</v>
+      </c>
+      <c r="D31" s="24" t="str">
+        <f ca="1"/>
+        <v>18:29:49</v>
+      </c>
+      <c r="E31" s="24" t="str">
+        <f ca="1"/>
+        <v>18:29:56</v>
+      </c>
+      <c r="F31" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G31" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H31" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I31" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J31" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="23" t="str">
         <f ca="1"/>
         <v>Global_Domination</v>
       </c>
-      <c r="C22" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D22" s="24" t="str">
-        <f ca="1"/>
-        <v>15:56:51</v>
-      </c>
-      <c r="E22" s="24">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="31">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G22" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="H22" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="I22" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="J22" s="32">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="23" t="str">
-        <f ca="1"/>
-        <v>Global_Domination</v>
-      </c>
-      <c r="C23" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D23" s="24" t="str">
-        <f ca="1"/>
-        <v>15:55:35</v>
-      </c>
-      <c r="E23" s="24">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="31">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G23" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="H23" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="I23" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="J23" s="32">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="23" t="str">
-        <f ca="1"/>
-        <v>Dino-Team</v>
-      </c>
-      <c r="C24" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D24" s="24" t="str">
-        <f ca="1"/>
-        <v>15:54:53</v>
-      </c>
-      <c r="E24" s="24">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="31">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G24" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="H24" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="I24" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="J24" s="32">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="23" t="str">
-        <f ca="1"/>
-        <v>Global_Domination</v>
-      </c>
-      <c r="C25" s="24" t="str">
-        <f ca="1"/>
-        <v>yap</v>
-      </c>
-      <c r="D25" s="24" t="str">
-        <f ca="1"/>
-        <v>15:54:40</v>
-      </c>
-      <c r="E25" s="24">
-        <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="31">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="G25" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="H25" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="I25" s="31">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-      <c r="J25" s="32">
-        <f ca="1"/>
-        <v>999</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="23" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="C26" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="D26" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="E26" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F26" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G26" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H26" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I26" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J26" s="32" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="23" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="C27" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="D27" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="E27" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F27" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G27" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H27" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I27" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J27" s="32" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="23" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="C28" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="D28" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="E28" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F28" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G28" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H28" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I28" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J28" s="32" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="23" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="C29" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="D29" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="E29" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F29" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G29" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H29" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I29" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J29" s="32" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="23" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="C30" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="D30" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="E30" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F30" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G30" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H30" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I30" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J30" s="32" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="23" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="C31" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="D31" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="E31" s="24" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F31" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G31" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H31" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I31" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J31" s="32" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="23" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
       <c r="C32" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D32" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>18:29:40</v>
       </c>
       <c r="E32" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F32" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G32" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H32" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I32" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J32" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>18:29:48</v>
+      </c>
+      <c r="F32" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G32" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H32" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I32" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J32" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>Global_Domination</v>
       </c>
       <c r="C33" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D33" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>18:28:15</v>
       </c>
       <c r="E33" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F33" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G33" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H33" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I33" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J33" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>18:28:24</v>
+      </c>
+      <c r="F33" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G33" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H33" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I33" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J33" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>emm</v>
       </c>
       <c r="C34" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D34" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>18:22:59</v>
       </c>
       <c r="E34" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F34" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G34" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H34" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I34" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J34" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>18:23:07</v>
+      </c>
+      <c r="F34" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G34" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H34" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I34" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J34" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>Global_Domination</v>
       </c>
       <c r="C35" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D35" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>18:21:19</v>
       </c>
       <c r="E35" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F35" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G35" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H35" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I35" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J35" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>18:21:27</v>
+      </c>
+      <c r="F35" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G35" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H35" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I35" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J35" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>emm</v>
       </c>
       <c r="C36" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D36" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>18:16:33</v>
       </c>
       <c r="E36" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F36" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G36" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H36" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I36" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J36" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>18:16:41</v>
+      </c>
+      <c r="F36" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G36" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H36" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I36" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J36" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B37" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>emm</v>
       </c>
       <c r="C37" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D37" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>18:16:01</v>
       </c>
       <c r="E37" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F37" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G37" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H37" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I37" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J37" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>18:16:11</v>
+      </c>
+      <c r="F37" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G37" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H37" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I37" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J37" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B38" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>emm</v>
       </c>
       <c r="C38" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D38" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>18:15:41</v>
       </c>
       <c r="E38" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F38" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G38" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H38" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I38" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J38" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>18:15:51</v>
+      </c>
+      <c r="F38" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G38" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H38" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I38" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J38" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>Dino-Team</v>
       </c>
       <c r="C39" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D39" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>18:15:07</v>
       </c>
       <c r="E39" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F39" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G39" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H39" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I39" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J39" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>18:15:16</v>
+      </c>
+      <c r="F39" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G39" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H39" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I39" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J39" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B40" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>Global_Domination</v>
       </c>
       <c r="C40" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D40" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>18:14:30</v>
       </c>
       <c r="E40" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F40" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G40" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H40" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I40" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J40" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>18:14:37</v>
+      </c>
+      <c r="F40" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G40" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H40" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I40" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J40" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>emm</v>
       </c>
       <c r="C41" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D41" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>18:13:05</v>
       </c>
       <c r="E41" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F41" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G41" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H41" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I41" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J41" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>18:13:14</v>
+      </c>
+      <c r="F41" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G41" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H41" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I41" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J41" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>Dino-Team</v>
       </c>
       <c r="C42" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D42" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>18:09:24</v>
       </c>
       <c r="E42" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F42" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G42" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H42" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I42" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J42" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>18:09:32</v>
+      </c>
+      <c r="F42" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G42" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H42" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I42" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J42" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>emm</v>
       </c>
       <c r="C43" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D43" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>17:48:08</v>
       </c>
       <c r="E43" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F43" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G43" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H43" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I43" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J43" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>17:48:16</v>
+      </c>
+      <c r="F43" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G43" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H43" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I43" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J43" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>emm</v>
       </c>
       <c r="C44" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D44" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>17:47:47</v>
       </c>
       <c r="E44" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F44" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G44" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H44" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I44" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J44" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>17:47:55</v>
+      </c>
+      <c r="F44" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G44" s="31">
+        <f ca="1"/>
+        <v>775475</v>
+      </c>
+      <c r="H44" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I44" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J44" s="32">
+        <f ca="1"/>
+        <v>25015.322580645163</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>draginoi</v>
       </c>
       <c r="C45" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D45" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>17:42:56</v>
       </c>
       <c r="E45" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F45" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G45" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H45" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I45" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J45" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>17:42:58</v>
+      </c>
+      <c r="F45" s="31">
+        <f ca="1"/>
+        <v>13</v>
+      </c>
+      <c r="G45" s="31">
+        <f ca="1"/>
+        <v>86348</v>
+      </c>
+      <c r="H45" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I45" s="31">
+        <f ca="1"/>
+        <v>86360</v>
+      </c>
+      <c r="J45" s="32">
+        <f ca="1"/>
+        <v>6642.1538461538457</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>draginoi</v>
       </c>
       <c r="C46" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D46" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>17:41:34</v>
       </c>
       <c r="E46" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F46" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G46" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H46" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I46" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J46" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>17:41:39</v>
+      </c>
+      <c r="F46" s="31">
+        <f ca="1"/>
+        <v>30</v>
+      </c>
+      <c r="G46" s="31">
+        <f ca="1"/>
+        <v>-30</v>
+      </c>
+      <c r="H46" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I46" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J46" s="32">
+        <f ca="1"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>emm</v>
       </c>
       <c r="C47" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D47" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>17:32:24</v>
       </c>
       <c r="E47" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F47" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G47" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H47" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I47" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J47" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>17:32:27</v>
+      </c>
+      <c r="F47" s="31">
+        <f ca="1"/>
+        <v>20</v>
+      </c>
+      <c r="G47" s="31">
+        <f ca="1"/>
+        <v>-20</v>
+      </c>
+      <c r="H47" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I47" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J47" s="32">
+        <f ca="1"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>emm</v>
       </c>
       <c r="C48" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D48" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>17:29:29</v>
       </c>
       <c r="E48" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F48" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G48" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H48" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I48" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J48" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>17:29:32</v>
+      </c>
+      <c r="F48" s="31">
+        <f ca="1"/>
+        <v>19</v>
+      </c>
+      <c r="G48" s="31">
+        <f ca="1"/>
+        <v>-19</v>
+      </c>
+      <c r="H48" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="I48" s="31">
+        <f ca="1"/>
+        <v>-1</v>
+      </c>
+      <c r="J48" s="32">
+        <f ca="1"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B49" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>emm</v>
       </c>
       <c r="C49" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D49" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>17:18:31</v>
       </c>
       <c r="E49" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F49" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G49" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H49" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I49" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J49" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>17:18:41</v>
+      </c>
+      <c r="F49" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G49" s="31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="H49" s="31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="I49" s="31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="32">
+        <f ca="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B50" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>emm</v>
       </c>
       <c r="C50" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D50" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>17:17:19</v>
       </c>
       <c r="E50" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F50" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G50" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H50" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I50" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J50" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>17:17:19</v>
+      </c>
+      <c r="F50" s="31">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="G50" s="31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="H50" s="31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="I50" s="31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="32">
+        <f ca="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B51" s="23" t="str">
         <f ca="1"/>
-        <v/>
+        <v>emm</v>
       </c>
       <c r="C51" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>sched</v>
       </c>
       <c r="D51" s="24" t="str">
         <f ca="1"/>
-        <v/>
+        <v>17:14:37</v>
       </c>
       <c r="E51" s="24" t="str">
         <f ca="1"/>
-        <v/>
-      </c>
-      <c r="F51" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="G51" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="H51" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="I51" s="31" t="str">
-        <f ca="1"/>
-        <v/>
-      </c>
-      <c r="J51" s="32" t="str">
-        <f ca="1"/>
-        <v/>
+        <v>17:14:41</v>
+      </c>
+      <c r="F51" s="31">
+        <f ca="1"/>
+        <v>31</v>
+      </c>
+      <c r="G51" s="31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="H51" s="31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="I51" s="31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="J51" s="32">
+        <f ca="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">

</xml_diff>